<commit_message>
fix: Error in tabulation of Miles McElhany Scoring
</commit_message>
<xml_diff>
--- a/static/downloads/2021/WMRRA-2021-Points-as-of-080321.xlsx
+++ b/static/downloads/2021/WMRRA-2021-Points-as-of-080321.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MotoM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E02827B1-0047-45E3-98DD-2AF29BAD722F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D067186-4FE4-46FE-A76B-0613FCE241B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" xr2:uid="{58302ADD-EE14-46B2-B8AB-B8706E5B8C2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{58302ADD-EE14-46B2-B8AB-B8706E5B8C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 Championship" sheetId="1" r:id="rId1"/>
@@ -158,6 +158,9 @@
     <t>Garret Visser</t>
   </si>
   <si>
+    <t>Miles McElhany</t>
+  </si>
+  <si>
     <t>Andy Halbert</t>
   </si>
   <si>
@@ -171,9 +174,6 @@
   </si>
   <si>
     <t>Micah Kudo</t>
-  </si>
-  <si>
-    <t>Miles McElhany</t>
   </si>
   <si>
     <t>Dave Heinricks</t>
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:U95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2:U95"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
@@ -2310,34 +2310,42 @@
         <v>11</v>
       </c>
       <c r="B12" s="117">
-        <v>107</v>
+        <v>343</v>
       </c>
       <c r="C12" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="43">
+        <v>14</v>
+      </c>
+      <c r="E12" s="43">
+        <v>42</v>
+      </c>
       <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44">
-        <v>89.5</v>
-      </c>
-      <c r="M12" s="44"/>
-      <c r="N12" s="36">
-        <v>128</v>
-      </c>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="47"/>
+      <c r="G12" s="43">
+        <v>17</v>
+      </c>
+      <c r="H12" s="42">
+        <v>71</v>
+      </c>
+      <c r="I12" s="42">
+        <v>43</v>
+      </c>
+      <c r="J12" s="42"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45">
+        <v>147</v>
+      </c>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="48"/>
       <c r="T12" s="38">
-        <f>128+89.5</f>
-        <v>217.5</v>
+        <f>147+71</f>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -2346,32 +2354,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="117">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="C13" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="43"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="44">
-        <v>203.5</v>
-      </c>
-      <c r="R13" s="43"/>
-      <c r="S13" s="58"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44">
+        <v>89.5</v>
+      </c>
+      <c r="M13" s="44"/>
+      <c r="N13" s="36">
+        <v>128</v>
+      </c>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="47"/>
       <c r="T13" s="38">
-        <f>203.5</f>
-        <v>203.5</v>
+        <f>128+89.5</f>
+        <v>217.5</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -2380,34 +2390,32 @@
         <v>13</v>
       </c>
       <c r="B14" s="117">
-        <v>17</v>
-      </c>
-      <c r="C14" s="132" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="130" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="44">
-        <v>44.5</v>
-      </c>
-      <c r="M14" s="45"/>
-      <c r="N14" s="36">
-        <v>158.5</v>
-      </c>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="48"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="44">
+        <v>203.5</v>
+      </c>
+      <c r="R14" s="43"/>
+      <c r="S14" s="58"/>
       <c r="T14" s="38">
-        <f>158.5+44.5</f>
-        <v>203</v>
+        <f>203.5</f>
+        <v>203.5</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2416,36 +2424,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="117">
-        <v>82</v>
-      </c>
-      <c r="C15" s="130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="42">
-        <v>106</v>
-      </c>
+      <c r="D15" s="42"/>
       <c r="E15" s="43"/>
-      <c r="F15" s="42">
-        <v>84</v>
-      </c>
-      <c r="G15" s="44">
-        <v>55</v>
-      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="58"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="44">
+        <v>44.5</v>
+      </c>
+      <c r="M15" s="45"/>
+      <c r="N15" s="36">
+        <v>158.5</v>
+      </c>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="48"/>
       <c r="T15" s="38">
-        <f>106+84</f>
-        <v>190</v>
+        <f>158.5+44.5</f>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2454,36 +2460,36 @@
         <v>15</v>
       </c>
       <c r="B16" s="117">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43">
-        <v>87</v>
-      </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="42">
-        <v>95</v>
-      </c>
-      <c r="I16" s="44">
-        <v>94</v>
-      </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
+      <c r="D16" s="42">
+        <v>106</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="42">
+        <v>84</v>
+      </c>
+      <c r="G16" s="44">
+        <v>55</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
       <c r="N16" s="36"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="47"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="58"/>
       <c r="T16" s="38">
-        <f>95+94</f>
-        <v>189</v>
+        <f>106+84</f>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -2492,42 +2498,36 @@
         <v>16</v>
       </c>
       <c r="B17" s="117">
-        <v>343</v>
+        <v>84</v>
       </c>
       <c r="C17" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="43">
-        <v>14</v>
-      </c>
+      <c r="D17" s="43"/>
       <c r="E17" s="43">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="F17" s="43"/>
-      <c r="G17" s="43">
-        <v>17</v>
-      </c>
+      <c r="G17" s="43"/>
       <c r="H17" s="42">
-        <v>71</v>
-      </c>
-      <c r="I17" s="42">
-        <v>43</v>
-      </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
+        <v>95</v>
+      </c>
+      <c r="I17" s="44">
+        <v>94</v>
+      </c>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
       <c r="N17" s="36"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45">
-        <v>117</v>
-      </c>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="48"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="44"/>
+      <c r="S17" s="47"/>
       <c r="T17" s="38">
-        <f>117+71</f>
-        <v>188</v>
+        <f>95+94</f>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -5464,7 +5464,7 @@
         <v>107</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="8">
         <f>31+17+41.5</f>
@@ -5548,7 +5548,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="8">
         <f>14.5+13+17</f>
@@ -5864,7 +5864,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="144" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="32">
         <f>18.5+32+35+29+44</f>
@@ -5876,7 +5876,7 @@
         <v>107</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="13">
         <f>41+45+42</f>
@@ -6230,7 +6230,7 @@
         <v>343</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D4" s="29">
         <f>40+29+42+36</f>
@@ -6365,7 +6365,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="139">
         <f>25+42.5+45.5+44.5+46</f>
@@ -7341,7 +7341,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="9">
         <f>18+15+21+34+18</f>
@@ -7413,7 +7413,7 @@
         <v>343</v>
       </c>
       <c r="C18" s="78" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D18" s="13">
         <v>14</v>
@@ -7811,7 +7811,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="145">
         <f>14+30+22+8+13</f>
@@ -7907,7 +7907,7 @@
         <v>343</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="145">
         <f>10+19+12+1</f>
@@ -8269,7 +8269,7 @@
         <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="146">
         <f>13+16+10+29+16</f>
@@ -8499,7 +8499,7 @@
         <v>82</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="8">
         <f>13+10+21+11</f>
@@ -8535,7 +8535,7 @@
         <v>343</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D13" s="13">
         <f>5+12</f>
@@ -8706,7 +8706,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="9">
         <f>16+29+32+2+16</f>
@@ -8766,7 +8766,7 @@
         <v>343</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D13" s="9">
         <f>26+15+26+4</f>
@@ -9142,7 +9142,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="139">
         <f>22+45+15+12</f>
@@ -9238,7 +9238,7 @@
         <v>343</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="146">
         <f>19+11+13</f>

</xml_diff>